<commit_message>
kw 277 - 300
</commit_message>
<xml_diff>
--- a/PenerimaanSPP.xlsx
+++ b/PenerimaanSPP.xlsx
@@ -19,13 +19,13 @@
   <calcPr calcId="124519"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId5"/>
-    <pivotCache cacheId="3" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="254">
   <si>
     <t>No</t>
   </si>
@@ -779,6 +779,15 @@
   <si>
     <t>Muhammad Fakhrudin Mutsaqif</t>
   </si>
+  <si>
+    <t>Dipa Surya Purnama</t>
+  </si>
+  <si>
+    <t>Yahya bin Abu Musa</t>
+  </si>
+  <si>
+    <t>17/12/2016</t>
+  </si>
 </sst>
 </file>
 
@@ -829,7 +838,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -845,6 +854,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -25013,7 +25023,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B503" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -40869,8 +40879,8 @@
   <dimension ref="A1:AF1010"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A838" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A859" sqref="A859"/>
+      <pane ySplit="1" topLeftCell="A892" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O913" sqref="O913"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -44631,7 +44641,7 @@
         <v>101</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>65</v>
+        <v>252</v>
       </c>
       <c r="C80" s="2">
         <v>1</v>
@@ -46694,7 +46704,7 @@
         <v>130</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>103</v>
+        <v>251</v>
       </c>
       <c r="C123" s="2">
         <v>6</v>
@@ -48822,7 +48832,7 @@
         <v>159</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>103</v>
+        <v>251</v>
       </c>
       <c r="C168" s="2">
         <v>6</v>
@@ -50955,7 +50965,7 @@
         <v>309</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>103</v>
+        <v>251</v>
       </c>
       <c r="C213" s="2">
         <v>6</v>
@@ -53734,7 +53744,7 @@
         <v>365</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>103</v>
+        <v>251</v>
       </c>
       <c r="C272" s="2">
         <v>6</v>
@@ -63987,7 +63997,7 @@
         <v>42581</v>
       </c>
       <c r="E487" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F487" s="2">
         <v>2016</v>
@@ -81542,15 +81552,30 @@
       </c>
     </row>
     <row r="859" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A859" s="2">
+        <v>272</v>
+      </c>
+      <c r="B859" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C859">
+        <v>1</v>
+      </c>
       <c r="D859" s="8">
         <v>42655</v>
       </c>
+      <c r="E859" s="2">
+        <v>11</v>
+      </c>
       <c r="F859" s="2">
         <v>2016</v>
       </c>
+      <c r="G859" s="2">
+        <v>150000</v>
+      </c>
       <c r="H859">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I859">
         <f t="shared" si="9"/>
@@ -81574,15 +81599,30 @@
       </c>
     </row>
     <row r="860" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A860" s="2">
+        <v>272</v>
+      </c>
+      <c r="B860" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C860">
+        <v>1</v>
+      </c>
       <c r="D860" s="8">
         <v>42655</v>
       </c>
+      <c r="E860" s="2">
+        <v>12</v>
+      </c>
       <c r="F860" s="2">
         <v>2016</v>
       </c>
+      <c r="G860" s="2">
+        <v>150000</v>
+      </c>
       <c r="H860">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I860">
         <f t="shared" si="9"/>
@@ -81606,15 +81646,30 @@
       </c>
     </row>
     <row r="861" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A861" s="2">
+        <v>272</v>
+      </c>
+      <c r="B861" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C861">
+        <v>1</v>
+      </c>
       <c r="D861" s="8">
         <v>42655</v>
       </c>
+      <c r="E861" s="2">
+        <v>1</v>
+      </c>
       <c r="F861" s="2">
-        <v>2016</v>
+        <v>2017</v>
+      </c>
+      <c r="G861" s="2">
+        <v>150000</v>
       </c>
       <c r="H861">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I861">
         <f t="shared" si="9"/>
@@ -81638,27 +81693,42 @@
       </c>
     </row>
     <row r="862" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A862" s="2">
+        <v>273</v>
+      </c>
+      <c r="B862" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C862">
+        <v>6</v>
+      </c>
       <c r="D862" s="8">
         <v>42655</v>
       </c>
+      <c r="E862" s="2">
+        <v>12</v>
+      </c>
       <c r="F862" s="2">
         <v>2016</v>
       </c>
+      <c r="G862" s="2">
+        <v>425000</v>
+      </c>
       <c r="H862">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I862">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="J862">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K862">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P862" t="b">
         <f t="shared" si="4"/>
@@ -81670,15 +81740,30 @@
       </c>
     </row>
     <row r="863" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A863" s="2">
+        <v>274</v>
+      </c>
+      <c r="B863" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C863">
+        <v>2</v>
+      </c>
       <c r="D863" s="8">
         <v>42655</v>
       </c>
+      <c r="E863" s="2">
+        <v>12</v>
+      </c>
       <c r="F863" s="2">
         <v>2016</v>
       </c>
+      <c r="G863" s="2">
+        <v>100000</v>
+      </c>
       <c r="H863">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="I863">
         <f t="shared" si="9"/>
@@ -81702,12 +81787,30 @@
       </c>
     </row>
     <row r="864" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A864" s="2">
+        <v>274</v>
+      </c>
+      <c r="B864" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C864">
+        <v>5</v>
+      </c>
+      <c r="D864" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E864" s="2">
+        <v>12</v>
+      </c>
       <c r="F864" s="2">
         <v>2016</v>
       </c>
+      <c r="G864" s="2">
+        <v>100000</v>
+      </c>
       <c r="H864">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="I864">
         <f t="shared" si="9"/>
@@ -81727,28 +81830,46 @@
       </c>
       <c r="Q864" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="865" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="865" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A865" s="2">
+        <v>274</v>
+      </c>
+      <c r="B865" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C865">
+        <v>6</v>
+      </c>
+      <c r="D865" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E865" s="2">
+        <v>12</v>
+      </c>
       <c r="F865" s="2">
         <v>2016</v>
       </c>
+      <c r="G865" s="2">
+        <v>300000</v>
+      </c>
       <c r="H865">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I865">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J865">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K865">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P865" t="b">
         <f t="shared" si="4"/>
@@ -81756,28 +81877,46 @@
       </c>
       <c r="Q865" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="866" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="866" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A866" s="2">
+        <v>275</v>
+      </c>
+      <c r="B866" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C866">
+        <v>6</v>
+      </c>
+      <c r="D866" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E866" s="2">
+        <v>11</v>
+      </c>
       <c r="F866" s="2">
         <v>2016</v>
       </c>
+      <c r="G866" s="2">
+        <v>425000</v>
+      </c>
       <c r="H866">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I866">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="J866">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K866">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P866" t="b">
         <f t="shared" si="4"/>
@@ -81785,28 +81924,49 @@
       </c>
       <c r="Q866" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="867" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="867" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A867" s="2">
+        <v>276</v>
+      </c>
+      <c r="B867" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C867">
+        <v>11</v>
+      </c>
+      <c r="D867" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E867" s="2">
+        <v>12</v>
+      </c>
       <c r="F867" s="2">
         <v>2016</v>
       </c>
+      <c r="G867" s="2">
+        <v>435000</v>
+      </c>
       <c r="H867">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I867">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="J867">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K867">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10000</v>
+      </c>
+      <c r="L867">
+        <v>10000</v>
       </c>
       <c r="P867" t="b">
         <f t="shared" si="4"/>
@@ -81814,28 +81974,49 @@
       </c>
       <c r="Q867" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="868" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="868" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A868" s="2">
+        <v>276</v>
+      </c>
+      <c r="B868" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C868">
+        <v>9</v>
+      </c>
+      <c r="D868" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E868" s="2">
+        <v>12</v>
+      </c>
       <c r="F868" s="2">
         <v>2016</v>
       </c>
+      <c r="G868" s="2">
+        <v>435000</v>
+      </c>
       <c r="H868">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I868">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="J868">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K868">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10000</v>
+      </c>
+      <c r="L868">
+        <v>10000</v>
       </c>
       <c r="P868" t="b">
         <f t="shared" si="4"/>
@@ -81843,28 +82024,49 @@
       </c>
       <c r="Q868" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="869" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="869" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A869" s="2">
+        <v>276</v>
+      </c>
+      <c r="B869" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C869">
+        <v>6</v>
+      </c>
+      <c r="D869" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E869" s="2">
+        <v>12</v>
+      </c>
       <c r="F869" s="2">
         <v>2016</v>
       </c>
+      <c r="G869" s="2">
+        <v>435000</v>
+      </c>
       <c r="H869">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I869">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="J869">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K869">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10000</v>
+      </c>
+      <c r="L869">
+        <v>10000</v>
       </c>
       <c r="P869" t="b">
         <f t="shared" si="4"/>
@@ -81872,16 +82074,34 @@
       </c>
       <c r="Q869" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="870" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="870" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A870" s="2">
+        <v>278</v>
+      </c>
+      <c r="B870" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C870">
+        <v>4</v>
+      </c>
+      <c r="D870" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E870" s="2">
+        <v>11</v>
+      </c>
       <c r="F870" s="2">
         <v>2016</v>
       </c>
+      <c r="G870" s="2">
+        <v>150000</v>
+      </c>
       <c r="H870">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I870">
         <f t="shared" si="9"/>
@@ -81901,16 +82121,34 @@
       </c>
       <c r="Q870" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="871" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="871" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A871" s="2">
+        <v>278</v>
+      </c>
+      <c r="B871" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C871">
+        <v>1</v>
+      </c>
+      <c r="D871" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E871" s="2">
+        <v>11</v>
+      </c>
       <c r="F871" s="2">
         <v>2016</v>
       </c>
+      <c r="G871" s="2">
+        <v>150000</v>
+      </c>
       <c r="H871">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I871">
         <f t="shared" si="9"/>
@@ -81930,16 +82168,34 @@
       </c>
       <c r="Q871" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="872" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="872" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A872" s="2">
+        <v>278</v>
+      </c>
+      <c r="B872" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C872">
+        <v>4</v>
+      </c>
+      <c r="D872" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E872" s="2">
+        <v>12</v>
+      </c>
       <c r="F872" s="2">
         <v>2016</v>
       </c>
+      <c r="G872" s="2">
+        <v>150000</v>
+      </c>
       <c r="H872">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I872">
         <f t="shared" si="9"/>
@@ -81959,16 +82215,34 @@
       </c>
       <c r="Q872" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="873" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="873" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A873" s="2">
+        <v>278</v>
+      </c>
+      <c r="B873" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C873">
+        <v>1</v>
+      </c>
+      <c r="D873" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E873" s="2">
+        <v>12</v>
+      </c>
       <c r="F873" s="2">
         <v>2016</v>
       </c>
+      <c r="G873" s="2">
+        <v>150000</v>
+      </c>
       <c r="H873">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I873">
         <f t="shared" si="9"/>
@@ -81988,16 +82262,34 @@
       </c>
       <c r="Q873" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="874" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="874" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A874" s="2">
+        <v>279</v>
+      </c>
+      <c r="B874" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C874">
+        <v>3</v>
+      </c>
+      <c r="D874" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E874" s="2">
+        <v>11</v>
+      </c>
       <c r="F874" s="2">
         <v>2016</v>
       </c>
+      <c r="G874" s="2">
+        <v>100000</v>
+      </c>
       <c r="H874">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="I874">
         <f t="shared" si="9"/>
@@ -82017,16 +82309,34 @@
       </c>
       <c r="Q874" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="875" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="875" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A875" s="2">
+        <v>279</v>
+      </c>
+      <c r="B875" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C875">
+        <v>3</v>
+      </c>
+      <c r="D875" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E875" s="2">
+        <v>12</v>
+      </c>
       <c r="F875" s="2">
         <v>2016</v>
       </c>
+      <c r="G875" s="2">
+        <v>100000</v>
+      </c>
       <c r="H875">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="I875">
         <f t="shared" si="9"/>
@@ -82046,16 +82356,34 @@
       </c>
       <c r="Q875" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="876" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="876" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A876" s="2">
+        <v>279</v>
+      </c>
+      <c r="B876" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C876">
+        <v>3</v>
+      </c>
+      <c r="D876" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E876" s="2">
+        <v>11</v>
+      </c>
       <c r="F876" s="2">
         <v>2016</v>
       </c>
+      <c r="G876" s="2">
+        <v>100000</v>
+      </c>
       <c r="H876">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="I876">
         <f t="shared" si="9"/>
@@ -82075,16 +82403,34 @@
       </c>
       <c r="Q876" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="877" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="877" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A877" s="2">
+        <v>279</v>
+      </c>
+      <c r="B877" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C877">
+        <v>3</v>
+      </c>
+      <c r="D877" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E877" s="2">
+        <v>12</v>
+      </c>
       <c r="F877" s="2">
         <v>2016</v>
       </c>
+      <c r="G877" s="2">
+        <v>100000</v>
+      </c>
       <c r="H877">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="I877">
         <f t="shared" si="9"/>
@@ -82104,16 +82450,34 @@
       </c>
       <c r="Q877" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="878" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="878" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A878" s="2">
+        <v>280</v>
+      </c>
+      <c r="B878" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C878">
+        <v>2</v>
+      </c>
+      <c r="D878" s="8">
+        <v>42686</v>
+      </c>
+      <c r="E878" s="2">
+        <v>11</v>
+      </c>
       <c r="F878" s="2">
         <v>2016</v>
       </c>
+      <c r="G878" s="2">
+        <v>150000</v>
+      </c>
       <c r="H878">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I878">
         <f t="shared" si="9"/>
@@ -82133,16 +82497,34 @@
       </c>
       <c r="Q878" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="879" spans="6:17" ht="15.75" customHeight="1">
+        <v>201611</v>
+      </c>
+    </row>
+    <row r="879" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A879" s="2">
+        <v>281</v>
+      </c>
+      <c r="B879" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C879">
+        <v>3</v>
+      </c>
+      <c r="D879" s="8">
+        <v>42716</v>
+      </c>
+      <c r="E879" s="2">
+        <v>12</v>
+      </c>
       <c r="F879" s="2">
         <v>2016</v>
       </c>
+      <c r="G879" s="2">
+        <v>150000</v>
+      </c>
       <c r="H879">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I879">
         <f t="shared" si="9"/>
@@ -82162,16 +82544,34 @@
       </c>
       <c r="Q879" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="880" spans="6:17" ht="15.75" customHeight="1">
+        <v>201612</v>
+      </c>
+    </row>
+    <row r="880" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A880" s="2">
+        <v>282</v>
+      </c>
+      <c r="B880" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C880">
+        <v>5</v>
+      </c>
+      <c r="D880" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E880" s="2">
+        <v>11</v>
+      </c>
       <c r="F880" s="2">
         <v>2016</v>
       </c>
+      <c r="G880" s="2">
+        <v>175000</v>
+      </c>
       <c r="H880">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I880">
         <f t="shared" si="9"/>
@@ -82185,22 +82585,43 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="N880">
+        <v>25000</v>
+      </c>
       <c r="P880" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q880" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="881" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="881" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A881" s="2">
+        <v>282</v>
+      </c>
+      <c r="B881" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C881">
+        <v>5</v>
+      </c>
+      <c r="D881" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E881" s="2">
+        <v>12</v>
+      </c>
       <c r="F881" s="2">
         <v>2016</v>
       </c>
+      <c r="G881" s="2">
+        <v>175000</v>
+      </c>
       <c r="H881">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I881">
         <f t="shared" si="9"/>
@@ -82214,22 +82635,43 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="N881">
+        <v>25000</v>
+      </c>
       <c r="P881" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q881" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="882" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="882" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A882" s="2">
+        <v>282</v>
+      </c>
+      <c r="B882" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C882">
+        <v>3</v>
+      </c>
+      <c r="D882" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E882" s="2">
+        <v>11</v>
+      </c>
       <c r="F882" s="2">
         <v>2016</v>
       </c>
+      <c r="G882" s="2">
+        <v>175000</v>
+      </c>
       <c r="H882">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I882">
         <f t="shared" si="9"/>
@@ -82243,22 +82685,43 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="N882">
+        <v>25000</v>
+      </c>
       <c r="P882" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q882" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="883" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="883" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A883" s="2">
+        <v>282</v>
+      </c>
+      <c r="B883" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C883">
+        <v>3</v>
+      </c>
+      <c r="D883" s="8">
+        <v>42655</v>
+      </c>
+      <c r="E883" s="2">
+        <v>12</v>
+      </c>
       <c r="F883" s="2">
         <v>2016</v>
       </c>
+      <c r="G883" s="2">
+        <v>175000</v>
+      </c>
       <c r="H883">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I883">
         <f t="shared" si="9"/>
@@ -82272,22 +82735,43 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="N883">
+        <v>25000</v>
+      </c>
       <c r="P883" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q883" t="str">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="884" spans="6:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="884" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A884" s="2">
+        <v>285</v>
+      </c>
+      <c r="B884" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C884">
+        <v>2</v>
+      </c>
+      <c r="D884" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E884" s="2">
+        <v>12</v>
+      </c>
       <c r="F884" s="2">
         <v>2016</v>
       </c>
+      <c r="G884" s="2">
+        <v>150000</v>
+      </c>
       <c r="H884">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I884">
         <f t="shared" si="9"/>
@@ -82305,47 +82789,83 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q884" t="str">
+      <c r="Q884" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="885" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="885" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A885" s="2">
+        <v>285</v>
+      </c>
+      <c r="B885" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C885">
+        <v>9</v>
+      </c>
+      <c r="D885" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E885" s="2">
+        <v>12</v>
+      </c>
       <c r="F885" s="2">
         <v>2016</v>
       </c>
+      <c r="G885" s="2">
+        <v>425000</v>
+      </c>
       <c r="H885">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I885">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="J885">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K885">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P885" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q885" t="str">
+      <c r="Q885" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="886" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="886" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A886" s="2">
+        <v>286</v>
+      </c>
+      <c r="B886" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C886">
+        <v>4</v>
+      </c>
+      <c r="D886" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E886" s="2">
+        <v>12</v>
+      </c>
       <c r="F886" s="2">
         <v>2016</v>
       </c>
+      <c r="G886" s="2">
+        <v>150000</v>
+      </c>
       <c r="H886">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I886">
         <f t="shared" si="9"/>
@@ -82363,18 +82883,36 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q886" t="str">
+      <c r="Q886" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="887" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="887" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A887" s="2">
+        <v>287</v>
+      </c>
+      <c r="B887" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C887">
+        <v>3</v>
+      </c>
+      <c r="D887" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E887" s="2">
+        <v>12</v>
+      </c>
       <c r="F887" s="2">
         <v>2016</v>
       </c>
+      <c r="G887" s="2">
+        <v>150000</v>
+      </c>
       <c r="H887">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I887">
         <f t="shared" si="9"/>
@@ -82392,47 +82930,83 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q887" t="str">
+      <c r="Q887" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="888" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="888" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A888" s="2">
+        <v>287</v>
+      </c>
+      <c r="B888" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C888">
+        <v>6</v>
+      </c>
+      <c r="D888" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E888" s="2">
+        <v>12</v>
+      </c>
       <c r="F888" s="2">
         <v>2016</v>
       </c>
+      <c r="G888" s="2">
+        <v>425000</v>
+      </c>
       <c r="H888">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I888">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="J888">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K888">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P888" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q888" t="str">
+      <c r="Q888" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="889" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="889" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A889" s="2">
+        <v>288</v>
+      </c>
+      <c r="B889" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C889">
+        <v>2</v>
+      </c>
+      <c r="D889" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E889" s="2">
+        <v>11</v>
+      </c>
       <c r="F889" s="2">
         <v>2016</v>
       </c>
+      <c r="G889" s="2">
+        <v>150000</v>
+      </c>
       <c r="H889">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I889">
         <f t="shared" si="9"/>
@@ -82450,47 +83024,83 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q889" t="str">
+      <c r="Q889" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="890" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="890" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A890" s="2">
+        <v>289</v>
+      </c>
+      <c r="B890" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C890">
+        <v>7</v>
+      </c>
+      <c r="D890" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E890" s="2">
+        <v>12</v>
+      </c>
       <c r="F890" s="2">
         <v>2016</v>
       </c>
+      <c r="G890" s="2">
+        <v>350000</v>
+      </c>
       <c r="H890">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I890">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>185000</v>
       </c>
       <c r="J890">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K890">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P890" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q890" t="str">
+      <c r="Q890" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="891" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="891" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A891" s="2">
+        <v>290</v>
+      </c>
+      <c r="B891" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C891">
+        <v>1</v>
+      </c>
+      <c r="D891" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E891" s="2">
+        <v>12</v>
+      </c>
       <c r="F891" s="2">
         <v>2016</v>
       </c>
+      <c r="G891" s="2">
+        <v>150000</v>
+      </c>
       <c r="H891">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I891">
         <f t="shared" si="9"/>
@@ -82508,18 +83118,36 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q891" t="str">
+      <c r="Q891" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="892" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="892" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A892" s="2">
+        <v>291</v>
+      </c>
+      <c r="B892" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C892">
+        <v>2</v>
+      </c>
+      <c r="D892" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E892" s="2">
+        <v>11</v>
+      </c>
       <c r="F892" s="2">
         <v>2016</v>
       </c>
+      <c r="G892" s="2">
+        <v>150000</v>
+      </c>
       <c r="H892">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I892">
         <f t="shared" si="9"/>
@@ -82537,18 +83165,36 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q892" t="str">
+      <c r="Q892" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="893" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="893" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A893" s="2">
+        <v>291</v>
+      </c>
+      <c r="B893" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C893">
+        <v>2</v>
+      </c>
+      <c r="D893" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E893" s="2">
+        <v>12</v>
+      </c>
       <c r="F893" s="2">
         <v>2016</v>
       </c>
+      <c r="G893" s="2">
+        <v>150000</v>
+      </c>
       <c r="H893">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I893">
         <f t="shared" si="9"/>
@@ -82566,18 +83212,36 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q893" t="str">
+      <c r="Q893" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="894" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="894" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A894" s="2">
+        <v>291</v>
+      </c>
+      <c r="B894" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C894">
+        <v>2</v>
+      </c>
+      <c r="D894" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E894" s="2">
+        <v>1</v>
+      </c>
       <c r="F894" s="2">
-        <v>2016</v>
+        <v>2017</v>
+      </c>
+      <c r="G894" s="2">
+        <v>150000</v>
       </c>
       <c r="H894">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I894">
         <f t="shared" si="9"/>
@@ -82595,18 +83259,36 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q894" t="str">
+      <c r="Q894" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="895" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="895" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A895" s="2">
+        <v>292</v>
+      </c>
+      <c r="B895" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C895">
+        <v>2</v>
+      </c>
+      <c r="D895" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E895" s="2">
+        <v>12</v>
+      </c>
       <c r="F895" s="2">
         <v>2016</v>
       </c>
+      <c r="G895" s="2">
+        <v>75000</v>
+      </c>
       <c r="H895">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>75000</v>
       </c>
       <c r="I895">
         <f t="shared" si="9"/>
@@ -82624,18 +83306,36 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q895" t="str">
+      <c r="Q895" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="896" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="896" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A896" s="2">
+        <v>292</v>
+      </c>
+      <c r="B896" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C896">
+        <v>2</v>
+      </c>
+      <c r="D896" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E896" s="2">
+        <v>1</v>
+      </c>
       <c r="F896" s="2">
-        <v>2016</v>
+        <v>2017</v>
+      </c>
+      <c r="G896" s="2">
+        <v>75000</v>
       </c>
       <c r="H896">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>75000</v>
       </c>
       <c r="I896">
         <f t="shared" si="9"/>
@@ -82653,18 +83353,36 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q896" t="str">
+      <c r="Q896" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="897" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="897" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A897" s="2">
+        <v>292</v>
+      </c>
+      <c r="B897" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C897">
+        <v>2</v>
+      </c>
+      <c r="D897" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E897" s="2">
+        <v>12</v>
+      </c>
       <c r="F897" s="2">
         <v>2016</v>
       </c>
+      <c r="G897" s="2">
+        <v>75000</v>
+      </c>
       <c r="H897">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>75000</v>
       </c>
       <c r="I897">
         <f t="shared" si="9"/>
@@ -82682,18 +83400,36 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q897" t="str">
+      <c r="Q897" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="898" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="898" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A898" s="2">
+        <v>292</v>
+      </c>
+      <c r="B898" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C898">
+        <v>2</v>
+      </c>
+      <c r="D898" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E898" s="2">
+        <v>1</v>
+      </c>
       <c r="F898" s="2">
-        <v>2016</v>
+        <v>2017</v>
+      </c>
+      <c r="G898" s="2">
+        <v>75000</v>
       </c>
       <c r="H898">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>75000</v>
       </c>
       <c r="I898">
         <f t="shared" si="9"/>
@@ -82711,47 +83447,83 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q898" t="str">
+      <c r="Q898" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="899" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="899" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A899" s="2">
+        <v>293</v>
+      </c>
+      <c r="B899" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C899" s="2">
+        <v>7</v>
+      </c>
+      <c r="D899" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E899" s="2">
+        <v>10</v>
+      </c>
       <c r="F899" s="2">
         <v>2016</v>
       </c>
+      <c r="G899" s="2">
+        <v>270000</v>
+      </c>
       <c r="H899">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I899">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>105000</v>
       </c>
       <c r="J899">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K899">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P899" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q899" t="str">
+      <c r="Q899" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="900" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="900" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A900" s="2">
+        <v>294</v>
+      </c>
+      <c r="B900" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C900">
+        <v>1</v>
+      </c>
+      <c r="D900" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E900" s="2">
+        <v>12</v>
+      </c>
       <c r="F900" s="2">
         <v>2016</v>
       </c>
+      <c r="G900" s="2">
+        <v>150000</v>
+      </c>
       <c r="H900">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I900">
         <f t="shared" si="9"/>
@@ -82769,47 +83541,83 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q900" t="str">
+      <c r="Q900" t="e">
         <f t="shared" si="35"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="901" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="901" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A901" s="2">
+        <v>295</v>
+      </c>
+      <c r="B901" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C901">
+        <v>6</v>
+      </c>
+      <c r="D901" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E901" s="2">
+        <v>12</v>
+      </c>
       <c r="F901" s="2">
         <v>2016</v>
       </c>
+      <c r="G901" s="2">
+        <v>350000</v>
+      </c>
       <c r="H901">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I901">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>185000</v>
       </c>
       <c r="J901">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K901">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P901" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q901" t="str">
+      <c r="Q901" t="e">
         <f t="shared" ref="Q901:Q964" si="36">CONCATENATE(YEAR(D901),MONTH(D901))</f>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="902" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="902" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A902" s="2">
+        <v>296</v>
+      </c>
+      <c r="B902" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C902">
+        <v>5</v>
+      </c>
+      <c r="D902" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E902" s="2">
+        <v>11</v>
+      </c>
       <c r="F902" s="2">
         <v>2016</v>
       </c>
+      <c r="G902" s="2">
+        <v>150000</v>
+      </c>
       <c r="H902">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I902">
         <f t="shared" si="9"/>
@@ -82827,18 +83635,36 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q902" t="str">
+      <c r="Q902" t="e">
         <f t="shared" si="36"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="903" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="903" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A903" s="2">
+        <v>297</v>
+      </c>
+      <c r="B903" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C903">
+        <v>2</v>
+      </c>
+      <c r="D903" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E903" s="2">
+        <v>12</v>
+      </c>
       <c r="F903" s="2">
         <v>2016</v>
       </c>
+      <c r="G903" s="2">
+        <v>160000</v>
+      </c>
       <c r="H903">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I903">
         <f t="shared" si="9"/>
@@ -82852,22 +83678,43 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="O903">
+        <v>10000</v>
+      </c>
       <c r="P903" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q903" t="str">
+      <c r="Q903" t="e">
         <f t="shared" si="36"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="904" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="904" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A904" s="2">
+        <v>297</v>
+      </c>
+      <c r="B904" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C904">
+        <v>2</v>
+      </c>
+      <c r="D904" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E904" s="2">
+        <v>12</v>
+      </c>
       <c r="F904" s="2">
         <v>2016</v>
       </c>
+      <c r="G904" s="2">
+        <v>160000</v>
+      </c>
       <c r="H904">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I904">
         <f t="shared" si="9"/>
@@ -82881,138 +83728,231 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="O904">
+        <v>10000</v>
+      </c>
       <c r="P904" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q904" t="str">
+      <c r="Q904" t="e">
         <f t="shared" si="36"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="905" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="905" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A905" s="2">
+        <v>298</v>
+      </c>
+      <c r="B905" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C905">
+        <v>9</v>
+      </c>
+      <c r="D905" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E905" s="2">
+        <v>9</v>
+      </c>
       <c r="F905" s="2">
         <v>2016</v>
       </c>
+      <c r="G905" s="2">
+        <v>425000</v>
+      </c>
       <c r="H905">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I905">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="J905">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K905">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P905" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q905" t="str">
+      <c r="Q905" t="e">
         <f t="shared" si="36"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="906" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="906" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A906" s="2">
+        <v>298</v>
+      </c>
+      <c r="B906" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C906">
+        <v>9</v>
+      </c>
+      <c r="D906" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E906" s="2">
+        <v>10</v>
+      </c>
       <c r="F906" s="2">
         <v>2016</v>
       </c>
+      <c r="G906" s="2">
+        <v>425000</v>
+      </c>
       <c r="H906">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I906">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="J906">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K906">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P906" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q906" t="str">
+      <c r="Q906" t="e">
         <f t="shared" si="36"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="907" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="907" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A907" s="2">
+        <v>298</v>
+      </c>
+      <c r="B907" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C907">
+        <v>9</v>
+      </c>
+      <c r="D907" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E907" s="2">
+        <v>11</v>
+      </c>
       <c r="F907" s="2">
         <v>2016</v>
       </c>
+      <c r="G907" s="2">
+        <v>425000</v>
+      </c>
       <c r="H907">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I907">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="J907">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K907">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P907" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q907" t="str">
+      <c r="Q907" t="e">
         <f t="shared" si="36"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="908" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="908" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A908" s="2">
+        <v>298</v>
+      </c>
+      <c r="B908" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C908">
+        <v>9</v>
+      </c>
+      <c r="D908" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E908" s="2">
+        <v>12</v>
+      </c>
       <c r="F908" s="2">
         <v>2016</v>
       </c>
+      <c r="G908" s="2">
+        <v>425000</v>
+      </c>
       <c r="H908">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I908">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="J908">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K908">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P908" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q908" t="str">
+      <c r="Q908" t="e">
         <f t="shared" si="36"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="909" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="909" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A909" s="2">
+        <v>300</v>
+      </c>
+      <c r="B909" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C909">
+        <v>2</v>
+      </c>
+      <c r="D909" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E909" s="2">
+        <v>12</v>
+      </c>
       <c r="F909" s="2">
         <v>2016</v>
       </c>
+      <c r="G909" s="2">
+        <v>200000</v>
+      </c>
       <c r="H909">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I909">
         <f t="shared" si="9"/>
@@ -83026,16 +83966,19 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="O909">
+        <v>50000</v>
+      </c>
       <c r="P909" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q909" t="str">
+      <c r="Q909" t="e">
         <f t="shared" si="36"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="910" spans="6:17" ht="15.75" customHeight="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="910" spans="1:17" ht="15.75" customHeight="1">
       <c r="F910" s="2">
         <v>2016</v>
       </c>
@@ -83064,7 +84007,7 @@
         <v>19001</v>
       </c>
     </row>
-    <row r="911" spans="6:17" ht="15.75" customHeight="1">
+    <row r="911" spans="1:17" ht="15.75" customHeight="1">
       <c r="F911" s="2">
         <v>2016</v>
       </c>
@@ -83093,7 +84036,7 @@
         <v>19001</v>
       </c>
     </row>
-    <row r="912" spans="6:17" ht="15.75" customHeight="1">
+    <row r="912" spans="1:17" ht="15.75" customHeight="1">
       <c r="F912" s="2">
         <v>2016</v>
       </c>

</xml_diff>

<commit_message>
spp urwah dan uthbah
</commit_message>
<xml_diff>
--- a/PenerimaanSPP.xlsx
+++ b/PenerimaanSPP.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sep 2016" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sep 2016'!$A$1:$Q$1334</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sep 2016'!$A$1:$Q$1332</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
   <pivotCaches>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="228">
   <si>
     <t>Count of SPP</t>
   </si>
@@ -697,6 +697,15 @@
   <si>
     <t>Column Labels</t>
   </si>
+  <si>
+    <t>Malvino</t>
+  </si>
+  <si>
+    <t>MUH</t>
+  </si>
+  <si>
+    <t>Arfan</t>
+  </si>
 </sst>
 </file>
 
@@ -716,12 +725,12 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -33375,16 +33384,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF1334"/>
+  <dimension ref="A1:AF1332"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1228" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1250" sqref="F1250"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" customWidth="1"/>
     <col min="5" max="5" width="6.140625" customWidth="1"/>
@@ -38671,7 +38680,7 @@
         <v>122</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C112" s="2">
         <v>5</v>
@@ -90169,7 +90178,7 @@
         <v>425000</v>
       </c>
       <c r="H1198">
-        <f t="shared" ref="H1198:H1262" si="67">IF(C1198&lt;6,IF(E1198&lt;1,0,IF(G1198&gt;150000,150000,G1198)),150000)</f>
+        <f t="shared" ref="H1198:H1261" si="67">IF(C1198&lt;6,IF(E1198&lt;1,0,IF(G1198&gt;150000,150000,G1198)),150000)</f>
         <v>150000</v>
       </c>
       <c r="I1198">
@@ -91270,7 +91279,7 @@
         <v>1</v>
       </c>
       <c r="Q1221" t="str">
-        <f t="shared" ref="Q1221:Q1285" si="68">CONCATENATE(YEAR(D1221),MONTH(D1221))</f>
+        <f t="shared" ref="Q1221:Q1283" si="68">CONCATENATE(YEAR(D1221),MONTH(D1221))</f>
         <v>20173</v>
       </c>
     </row>
@@ -92463,7 +92472,7 @@
     </row>
     <row r="1247" spans="1:17" ht="15.75" customHeight="1">
       <c r="A1247">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B1247" s="2" t="s">
         <v>135</v>
@@ -92509,24 +92518,42 @@
       </c>
     </row>
     <row r="1248" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1248">
+        <v>867</v>
+      </c>
+      <c r="B1248" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1248" s="2">
+        <v>10</v>
+      </c>
       <c r="D1248" s="3">
         <v>42805</v>
       </c>
+      <c r="E1248" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1248" s="2">
+        <v>2017</v>
+      </c>
+      <c r="G1248" s="2">
+        <v>425000</v>
+      </c>
       <c r="H1248">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1248">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="J1248">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1248">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1248" t="b">
         <f t="shared" si="66"/>
@@ -92537,25 +92564,43 @@
         <v>20173</v>
       </c>
     </row>
-    <row r="1249" spans="4:17" ht="15.75" customHeight="1">
+    <row r="1249" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1249">
+        <v>868</v>
+      </c>
+      <c r="B1249" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1249" s="2">
+        <v>7</v>
+      </c>
       <c r="D1249" s="3">
         <v>42805</v>
       </c>
+      <c r="E1249" s="5">
+        <v>12</v>
+      </c>
+      <c r="F1249" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1249" s="2">
+        <v>425000</v>
+      </c>
       <c r="H1249">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1249">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="J1249">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1249">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1249" t="b">
         <f t="shared" si="66"/>
@@ -92566,25 +92611,43 @@
         <v>20173</v>
       </c>
     </row>
-    <row r="1250" spans="4:17" ht="15.75" customHeight="1">
+    <row r="1250" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1250">
+        <v>869</v>
+      </c>
+      <c r="B1250" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1250" s="2">
+        <v>7</v>
+      </c>
       <c r="D1250" s="3">
         <v>42805</v>
       </c>
+      <c r="E1250" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1250" s="2">
+        <v>2017</v>
+      </c>
+      <c r="G1250" s="2">
+        <v>425000</v>
+      </c>
       <c r="H1250">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1250">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="J1250">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1250">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1250" t="b">
         <f t="shared" si="66"/>
@@ -92595,25 +92658,43 @@
         <v>20173</v>
       </c>
     </row>
-    <row r="1251" spans="4:17" ht="15.75" customHeight="1">
+    <row r="1251" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1251">
+        <v>870</v>
+      </c>
+      <c r="B1251" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1251" s="2">
+        <v>7</v>
+      </c>
       <c r="D1251" s="3">
         <v>42805</v>
       </c>
+      <c r="E1251" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1251" s="2">
+        <v>2017</v>
+      </c>
+      <c r="G1251" s="2">
+        <v>425000</v>
+      </c>
       <c r="H1251">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1251">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="J1251">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1251">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1251" t="b">
         <f t="shared" si="66"/>
@@ -92624,13 +92705,31 @@
         <v>20173</v>
       </c>
     </row>
-    <row r="1252" spans="4:17" ht="15.75" customHeight="1">
+    <row r="1252" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1252">
+        <v>870</v>
+      </c>
+      <c r="B1252" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1252" s="2">
+        <v>4</v>
+      </c>
       <c r="D1252" s="3">
         <v>42805</v>
       </c>
+      <c r="E1252" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1252" s="2">
+        <v>2017</v>
+      </c>
+      <c r="G1252" s="2">
+        <v>150000</v>
+      </c>
       <c r="H1252">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1252">
         <f t="shared" si="63"/>
@@ -92653,13 +92752,31 @@
         <v>20173</v>
       </c>
     </row>
-    <row r="1253" spans="4:17" ht="15.75" customHeight="1">
+    <row r="1253" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1253">
+        <v>871</v>
+      </c>
+      <c r="B1253" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1253" s="2">
+        <v>3</v>
+      </c>
       <c r="D1253" s="3">
         <v>42805</v>
       </c>
+      <c r="E1253" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1253" s="2">
+        <v>2017</v>
+      </c>
+      <c r="G1253" s="2">
+        <v>150000</v>
+      </c>
       <c r="H1253">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1253">
         <f t="shared" si="63"/>
@@ -92682,13 +92799,31 @@
         <v>20173</v>
       </c>
     </row>
-    <row r="1254" spans="4:17" ht="15.75" customHeight="1">
+    <row r="1254" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1254">
+        <v>871</v>
+      </c>
+      <c r="B1254" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1254" s="2">
+        <v>5</v>
+      </c>
       <c r="D1254" s="3">
         <v>42805</v>
       </c>
+      <c r="E1254" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1254" s="2">
+        <v>2017</v>
+      </c>
+      <c r="G1254" s="2">
+        <v>150000</v>
+      </c>
       <c r="H1254">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1254">
         <f t="shared" si="63"/>
@@ -92711,13 +92846,31 @@
         <v>20173</v>
       </c>
     </row>
-    <row r="1255" spans="4:17" ht="15.75" customHeight="1">
+    <row r="1255" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1255">
+        <v>872</v>
+      </c>
+      <c r="B1255" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1255" s="2">
+        <v>2</v>
+      </c>
       <c r="D1255" s="3">
         <v>42805</v>
       </c>
+      <c r="E1255" s="2">
+        <v>2</v>
+      </c>
+      <c r="F1255" s="2">
+        <v>2017</v>
+      </c>
+      <c r="G1255" s="2">
+        <v>150000</v>
+      </c>
       <c r="H1255">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1255">
         <f t="shared" si="63"/>
@@ -92740,13 +92893,31 @@
         <v>20173</v>
       </c>
     </row>
-    <row r="1256" spans="4:17" ht="15.75" customHeight="1">
+    <row r="1256" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1256">
+        <v>872</v>
+      </c>
+      <c r="B1256" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1256" s="2">
+        <v>2</v>
+      </c>
       <c r="D1256" s="3">
         <v>42805</v>
       </c>
+      <c r="E1256" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1256" s="2">
+        <v>2017</v>
+      </c>
+      <c r="G1256" s="2">
+        <v>150000</v>
+      </c>
       <c r="H1256">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1256">
         <f t="shared" si="63"/>
@@ -92769,25 +92940,43 @@
         <v>20173</v>
       </c>
     </row>
-    <row r="1257" spans="4:17" ht="15.75" customHeight="1">
-      <c r="D1257" s="3">
-        <v>42805</v>
+    <row r="1257" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1257" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1257" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1257" s="2">
+        <v>9</v>
+      </c>
+      <c r="D1257" s="9">
+        <v>42605</v>
+      </c>
+      <c r="E1257" s="2">
+        <v>8</v>
+      </c>
+      <c r="F1257" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1257" s="2">
+        <v>300000</v>
       </c>
       <c r="H1257">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1257">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1257">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1257">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1257" t="b">
         <f t="shared" si="66"/>
@@ -92795,28 +92984,46 @@
       </c>
       <c r="Q1257" t="str">
         <f t="shared" si="68"/>
-        <v>20173</v>
-      </c>
-    </row>
-    <row r="1258" spans="4:17" ht="15.75" customHeight="1">
-      <c r="D1258" s="3">
-        <v>42805</v>
+        <v>20168</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1258" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1258" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1258" s="2">
+        <v>9</v>
+      </c>
+      <c r="D1258" s="9">
+        <v>42636</v>
+      </c>
+      <c r="E1258" s="2">
+        <v>9</v>
+      </c>
+      <c r="F1258" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1258" s="2">
+        <v>300000</v>
       </c>
       <c r="H1258">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1258">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1258">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1258">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1258" t="b">
         <f t="shared" si="66"/>
@@ -92824,28 +93031,46 @@
       </c>
       <c r="Q1258" t="str">
         <f t="shared" si="68"/>
-        <v>20173</v>
-      </c>
-    </row>
-    <row r="1259" spans="4:17" ht="15.75" customHeight="1">
-      <c r="D1259" s="3">
-        <v>42805</v>
+        <v>20169</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1259" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1259" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1259" s="2">
+        <v>9</v>
+      </c>
+      <c r="D1259" s="9">
+        <v>42666</v>
+      </c>
+      <c r="E1259" s="2">
+        <v>10</v>
+      </c>
+      <c r="F1259" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1259" s="2">
+        <v>300000</v>
       </c>
       <c r="H1259">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1259">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1259">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1259">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1259" t="b">
         <f t="shared" si="66"/>
@@ -92853,28 +93078,46 @@
       </c>
       <c r="Q1259" t="str">
         <f t="shared" si="68"/>
-        <v>20173</v>
-      </c>
-    </row>
-    <row r="1260" spans="4:17" ht="15.75" customHeight="1">
-      <c r="D1260" s="3">
-        <v>42805</v>
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1260" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1260" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1260" s="2">
+        <v>9</v>
+      </c>
+      <c r="D1260" s="9">
+        <v>42697</v>
+      </c>
+      <c r="E1260" s="2">
+        <v>11</v>
+      </c>
+      <c r="F1260" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1260" s="2">
+        <v>300000</v>
       </c>
       <c r="H1260">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1260">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1260">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1260">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1260" t="b">
         <f t="shared" si="66"/>
@@ -92882,57 +93125,93 @@
       </c>
       <c r="Q1260" t="str">
         <f t="shared" si="68"/>
-        <v>20173</v>
-      </c>
-    </row>
-    <row r="1261" spans="4:17" ht="15.75" customHeight="1">
-      <c r="D1261" s="3">
-        <v>42805</v>
+        <v>201611</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1261" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1261" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1261" s="2">
+        <v>9</v>
+      </c>
+      <c r="D1261" s="9">
+        <v>42727</v>
+      </c>
+      <c r="E1261" s="2">
+        <v>12</v>
+      </c>
+      <c r="F1261" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1261" s="2">
+        <v>300000</v>
       </c>
       <c r="H1261">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1261">
-        <f t="shared" ref="I1261:I1324" si="75">IF(C1261&lt;6,0,G1261-H1261-SUM(J1261:O1261))</f>
-        <v>0</v>
+        <f t="shared" ref="I1261:I1322" si="75">IF(C1261&lt;6,0,G1261-H1261-SUM(J1261:O1261))</f>
+        <v>135000</v>
       </c>
       <c r="J1261">
-        <f t="shared" ref="J1261:J1324" si="76">IF(C1261&lt;6,0,5000)</f>
-        <v>0</v>
+        <f t="shared" ref="J1261:J1322" si="76">IF(C1261&lt;6,0,5000)</f>
+        <v>5000</v>
       </c>
       <c r="K1261">
-        <f t="shared" ref="K1261:K1324" si="77">IF(C1261&lt;6,0,10000)</f>
-        <v>0</v>
+        <f t="shared" ref="K1261:K1322" si="77">IF(C1261&lt;6,0,10000)</f>
+        <v>10000</v>
       </c>
       <c r="P1261" t="b">
-        <f t="shared" ref="P1261:P1324" si="78">G1261=SUM(H1261:O1261)</f>
+        <f t="shared" ref="P1261:P1322" si="78">G1261=SUM(H1261:O1261)</f>
         <v>1</v>
       </c>
       <c r="Q1261" t="str">
         <f t="shared" si="68"/>
-        <v>20173</v>
-      </c>
-    </row>
-    <row r="1262" spans="4:17" ht="15.75" customHeight="1">
-      <c r="D1262" s="3">
-        <v>42805</v>
+        <v>201612</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1262" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1262" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1262" s="2">
+        <v>11</v>
+      </c>
+      <c r="D1262" s="9">
+        <v>42605</v>
+      </c>
+      <c r="E1262" s="2">
+        <v>8</v>
+      </c>
+      <c r="F1262" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1262" s="2">
+        <v>300000</v>
       </c>
       <c r="H1262">
-        <f t="shared" si="67"/>
-        <v>0</v>
+        <f t="shared" ref="H1262:H1324" si="79">IF(C1262&lt;6,IF(E1262&lt;1,0,IF(G1262&gt;150000,150000,G1262)),150000)</f>
+        <v>150000</v>
       </c>
       <c r="I1262">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1262">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1262">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1262" t="b">
         <f t="shared" si="78"/>
@@ -92940,28 +93219,46 @@
       </c>
       <c r="Q1262" t="str">
         <f t="shared" si="68"/>
-        <v>20173</v>
-      </c>
-    </row>
-    <row r="1263" spans="4:17" ht="15.75" customHeight="1">
-      <c r="D1263" s="3">
-        <v>42805</v>
+        <v>20168</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1263" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1263" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1263" s="2">
+        <v>11</v>
+      </c>
+      <c r="D1263" s="9">
+        <v>42636</v>
+      </c>
+      <c r="E1263" s="2">
+        <v>9</v>
+      </c>
+      <c r="F1263" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1263" s="2">
+        <v>300000</v>
       </c>
       <c r="H1263">
-        <f t="shared" ref="H1263:H1326" si="79">IF(C1263&lt;6,IF(E1263&lt;1,0,IF(G1263&gt;150000,150000,G1263)),150000)</f>
-        <v>0</v>
+        <f t="shared" si="79"/>
+        <v>150000</v>
       </c>
       <c r="I1263">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1263">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1263">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1263" t="b">
         <f t="shared" si="78"/>
@@ -92969,28 +93266,46 @@
       </c>
       <c r="Q1263" t="str">
         <f t="shared" si="68"/>
-        <v>20173</v>
-      </c>
-    </row>
-    <row r="1264" spans="4:17" ht="15.75" customHeight="1">
-      <c r="D1264" s="3">
-        <v>42805</v>
+        <v>20169</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1264" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1264" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1264" s="2">
+        <v>11</v>
+      </c>
+      <c r="D1264" s="9">
+        <v>42666</v>
+      </c>
+      <c r="E1264" s="2">
+        <v>10</v>
+      </c>
+      <c r="F1264" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1264" s="2">
+        <v>300000</v>
       </c>
       <c r="H1264">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1264">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1264">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1264">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1264" t="b">
         <f t="shared" si="78"/>
@@ -92998,28 +93313,46 @@
       </c>
       <c r="Q1264" t="str">
         <f t="shared" si="68"/>
-        <v>20173</v>
-      </c>
-    </row>
-    <row r="1265" spans="4:17" ht="15.75" customHeight="1">
-      <c r="D1265" s="3">
-        <v>42805</v>
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1265" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1265" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1265" s="2">
+        <v>11</v>
+      </c>
+      <c r="D1265" s="9">
+        <v>42697</v>
+      </c>
+      <c r="E1265" s="2">
+        <v>11</v>
+      </c>
+      <c r="F1265" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1265" s="2">
+        <v>300000</v>
       </c>
       <c r="H1265">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1265">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1265">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1265">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1265" t="b">
         <f t="shared" si="78"/>
@@ -93027,25 +93360,46 @@
       </c>
       <c r="Q1265" t="str">
         <f t="shared" si="68"/>
-        <v>20173</v>
-      </c>
-    </row>
-    <row r="1266" spans="4:17" ht="15.75" customHeight="1">
+        <v>201611</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1266" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1266" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1266" s="2">
+        <v>11</v>
+      </c>
+      <c r="D1266" s="9">
+        <v>42727</v>
+      </c>
+      <c r="E1266" s="2">
+        <v>12</v>
+      </c>
+      <c r="F1266" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1266" s="2">
+        <v>300000</v>
+      </c>
       <c r="H1266">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1266">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1266">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1266">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1266" t="b">
         <f t="shared" si="78"/>
@@ -93053,25 +93407,46 @@
       </c>
       <c r="Q1266" t="str">
         <f t="shared" si="68"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="1267" spans="4:17" ht="15.75" customHeight="1">
+        <v>201612</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1267" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1267" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1267" s="2">
+        <v>8</v>
+      </c>
+      <c r="D1267" s="9">
+        <v>42636</v>
+      </c>
+      <c r="E1267" s="2">
+        <v>9</v>
+      </c>
+      <c r="F1267" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1267" s="2">
+        <v>300000</v>
+      </c>
       <c r="H1267">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1267">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1267">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1267">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1267" t="b">
         <f t="shared" si="78"/>
@@ -93079,25 +93454,46 @@
       </c>
       <c r="Q1267" t="str">
         <f t="shared" si="68"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="1268" spans="4:17" ht="15.75" customHeight="1">
+        <v>20169</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1268" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1268" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1268" s="2">
+        <v>8</v>
+      </c>
+      <c r="D1268" s="9">
+        <v>42666</v>
+      </c>
+      <c r="E1268" s="2">
+        <v>10</v>
+      </c>
+      <c r="F1268" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1268" s="2">
+        <v>300000</v>
+      </c>
       <c r="H1268">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1268">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1268">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1268">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1268" t="b">
         <f t="shared" si="78"/>
@@ -93105,25 +93501,46 @@
       </c>
       <c r="Q1268" t="str">
         <f t="shared" si="68"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="1269" spans="4:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1269" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1269" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1269" s="2">
+        <v>8</v>
+      </c>
+      <c r="D1269" s="9">
+        <v>42697</v>
+      </c>
+      <c r="E1269" s="2">
+        <v>11</v>
+      </c>
+      <c r="F1269" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1269" s="2">
+        <v>300000</v>
+      </c>
       <c r="H1269">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1269">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1269">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1269">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1269" t="b">
         <f t="shared" si="78"/>
@@ -93131,25 +93548,46 @@
       </c>
       <c r="Q1269" t="str">
         <f t="shared" si="68"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="1270" spans="4:17" ht="15.75" customHeight="1">
+        <v>201611</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1270" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1270" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1270" s="2">
+        <v>8</v>
+      </c>
+      <c r="D1270" s="9">
+        <v>42727</v>
+      </c>
+      <c r="E1270" s="2">
+        <v>12</v>
+      </c>
+      <c r="F1270" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1270" s="2">
+        <v>300000</v>
+      </c>
       <c r="H1270">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1270">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1270">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1270">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1270" t="b">
         <f t="shared" si="78"/>
@@ -93157,25 +93595,46 @@
       </c>
       <c r="Q1270" t="str">
         <f t="shared" si="68"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="1271" spans="4:17" ht="15.75" customHeight="1">
+        <v>201612</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1271" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1271" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1271" s="2">
+        <v>7</v>
+      </c>
+      <c r="D1271" s="9">
+        <v>42574</v>
+      </c>
+      <c r="E1271" s="2">
+        <v>7</v>
+      </c>
+      <c r="F1271" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1271" s="2">
+        <v>300000</v>
+      </c>
       <c r="H1271">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1271">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1271">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1271">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1271" t="b">
         <f t="shared" si="78"/>
@@ -93183,25 +93642,46 @@
       </c>
       <c r="Q1271" t="str">
         <f t="shared" si="68"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="1272" spans="4:17" ht="15.75" customHeight="1">
+        <v>20167</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1272" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1272" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1272" s="2">
+        <v>7</v>
+      </c>
+      <c r="D1272" s="9">
+        <v>42605</v>
+      </c>
+      <c r="E1272" s="2">
+        <v>8</v>
+      </c>
+      <c r="F1272" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1272" s="2">
+        <v>300000</v>
+      </c>
       <c r="H1272">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1272">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1272">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1272">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1272" t="b">
         <f t="shared" si="78"/>
@@ -93209,25 +93689,46 @@
       </c>
       <c r="Q1272" t="str">
         <f t="shared" si="68"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="1273" spans="4:17" ht="15.75" customHeight="1">
+        <v>20168</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1273" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1273" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1273" s="2">
+        <v>7</v>
+      </c>
+      <c r="D1273" s="9">
+        <v>42636</v>
+      </c>
+      <c r="E1273" s="2">
+        <v>9</v>
+      </c>
+      <c r="F1273" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1273" s="2">
+        <v>300000</v>
+      </c>
       <c r="H1273">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1273">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1273">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1273">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1273" t="b">
         <f t="shared" si="78"/>
@@ -93235,25 +93736,46 @@
       </c>
       <c r="Q1273" t="str">
         <f t="shared" si="68"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="1274" spans="4:17" ht="15.75" customHeight="1">
+        <v>20169</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1274" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1274" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1274" s="2">
+        <v>7</v>
+      </c>
+      <c r="D1274" s="9">
+        <v>42666</v>
+      </c>
+      <c r="E1274" s="2">
+        <v>10</v>
+      </c>
+      <c r="F1274" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G1274" s="2">
+        <v>300000</v>
+      </c>
       <c r="H1274">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="I1274">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="J1274">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K1274">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P1274" t="b">
         <f t="shared" si="78"/>
@@ -93261,10 +93783,10 @@
       </c>
       <c r="Q1274" t="str">
         <f t="shared" si="68"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="1275" spans="4:17" ht="15.75" customHeight="1">
+        <v>201610</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:17" ht="15.75" customHeight="1">
       <c r="H1275">
         <f t="shared" si="79"/>
         <v>0</v>
@@ -93290,7 +93812,7 @@
         <v>19001</v>
       </c>
     </row>
-    <row r="1276" spans="4:17" ht="15.75" customHeight="1">
+    <row r="1276" spans="1:17" ht="15.75" customHeight="1">
       <c r="H1276">
         <f t="shared" si="79"/>
         <v>0</v>
@@ -93316,7 +93838,7 @@
         <v>19001</v>
       </c>
     </row>
-    <row r="1277" spans="4:17" ht="15.75" customHeight="1">
+    <row r="1277" spans="1:17" ht="15.75" customHeight="1">
       <c r="H1277">
         <f t="shared" si="79"/>
         <v>0</v>
@@ -93342,7 +93864,7 @@
         <v>19001</v>
       </c>
     </row>
-    <row r="1278" spans="4:17" ht="15.75" customHeight="1">
+    <row r="1278" spans="1:17" ht="15.75" customHeight="1">
       <c r="H1278">
         <f t="shared" si="79"/>
         <v>0</v>
@@ -93368,7 +93890,7 @@
         <v>19001</v>
       </c>
     </row>
-    <row r="1279" spans="4:17" ht="15.75" customHeight="1">
+    <row r="1279" spans="1:17" ht="15.75" customHeight="1">
       <c r="H1279">
         <f t="shared" si="79"/>
         <v>0</v>
@@ -93394,7 +93916,7 @@
         <v>19001</v>
       </c>
     </row>
-    <row r="1280" spans="4:17" ht="15.75" customHeight="1">
+    <row r="1280" spans="1:17" ht="15.75" customHeight="1">
       <c r="H1280">
         <f t="shared" si="79"/>
         <v>0</v>
@@ -93520,7 +94042,7 @@
         <v>1</v>
       </c>
       <c r="Q1284" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" ref="Q1284:Q1332" si="80">CONCATENATE(YEAR(D1284),MONTH(D1284))</f>
         <v>19001</v>
       </c>
     </row>
@@ -93546,7 +94068,7 @@
         <v>1</v>
       </c>
       <c r="Q1285" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="80"/>
         <v>19001</v>
       </c>
     </row>
@@ -93572,7 +94094,7 @@
         <v>1</v>
       </c>
       <c r="Q1286" t="str">
-        <f t="shared" ref="Q1286:Q1334" si="80">CONCATENATE(YEAR(D1286),MONTH(D1286))</f>
+        <f t="shared" si="80"/>
         <v>19001</v>
       </c>
     </row>
@@ -94518,19 +95040,19 @@
         <v>0</v>
       </c>
       <c r="I1323">
-        <f t="shared" si="75"/>
+        <f t="shared" ref="I1323:I1332" si="81">IF(C1323&lt;6,0,G1323-H1323-SUM(J1323:O1323))</f>
         <v>0</v>
       </c>
       <c r="J1323">
-        <f t="shared" si="76"/>
+        <f t="shared" ref="J1323:J1332" si="82">IF(C1323&lt;6,0,5000)</f>
         <v>0</v>
       </c>
       <c r="K1323">
-        <f t="shared" si="77"/>
+        <f t="shared" ref="K1323:K1332" si="83">IF(C1323&lt;6,0,10000)</f>
         <v>0</v>
       </c>
       <c r="P1323" t="b">
-        <f t="shared" si="78"/>
+        <f t="shared" ref="P1323:P1332" si="84">G1323=SUM(H1323:O1323)</f>
         <v>1</v>
       </c>
       <c r="Q1323" t="str">
@@ -94544,19 +95066,19 @@
         <v>0</v>
       </c>
       <c r="I1324">
-        <f t="shared" si="75"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="J1324">
-        <f t="shared" si="76"/>
+        <f t="shared" si="82"/>
         <v>0</v>
       </c>
       <c r="K1324">
-        <f t="shared" si="77"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="P1324" t="b">
-        <f t="shared" si="78"/>
+        <f t="shared" si="84"/>
         <v>1</v>
       </c>
       <c r="Q1324" t="str">
@@ -94566,23 +95088,23 @@
     </row>
     <row r="1325" spans="8:17" ht="15.75" customHeight="1">
       <c r="H1325">
-        <f t="shared" si="79"/>
+        <f t="shared" ref="H1325:H1332" si="85">IF(C1325&lt;6,IF(E1325&lt;1,0,IF(G1325&gt;150000,150000,G1325)),150000)</f>
         <v>0</v>
       </c>
       <c r="I1325">
-        <f t="shared" ref="I1325:I1334" si="81">IF(C1325&lt;6,0,G1325-H1325-SUM(J1325:O1325))</f>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="J1325">
-        <f t="shared" ref="J1325:J1334" si="82">IF(C1325&lt;6,0,5000)</f>
+        <f t="shared" si="82"/>
         <v>0</v>
       </c>
       <c r="K1325">
-        <f t="shared" ref="K1325:K1334" si="83">IF(C1325&lt;6,0,10000)</f>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="P1325" t="b">
-        <f t="shared" ref="P1325:P1334" si="84">G1325=SUM(H1325:O1325)</f>
+        <f t="shared" si="84"/>
         <v>1</v>
       </c>
       <c r="Q1325" t="str">
@@ -94592,7 +95114,7 @@
     </row>
     <row r="1326" spans="8:17" ht="15.75" customHeight="1">
       <c r="H1326">
-        <f t="shared" si="79"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="I1326">
@@ -94618,7 +95140,7 @@
     </row>
     <row r="1327" spans="8:17" ht="15.75" customHeight="1">
       <c r="H1327">
-        <f t="shared" ref="H1327:H1334" si="85">IF(C1327&lt;6,IF(E1327&lt;1,0,IF(G1327&gt;150000,150000,G1327)),150000)</f>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="I1327">
@@ -94772,60 +95294,8 @@
         <v>19001</v>
       </c>
     </row>
-    <row r="1333" spans="8:17" ht="15.75" customHeight="1">
-      <c r="H1333">
-        <f t="shared" si="85"/>
-        <v>0</v>
-      </c>
-      <c r="I1333">
-        <f t="shared" si="81"/>
-        <v>0</v>
-      </c>
-      <c r="J1333">
-        <f t="shared" si="82"/>
-        <v>0</v>
-      </c>
-      <c r="K1333">
-        <f t="shared" si="83"/>
-        <v>0</v>
-      </c>
-      <c r="P1333" t="b">
-        <f t="shared" si="84"/>
-        <v>1</v>
-      </c>
-      <c r="Q1333" t="str">
-        <f t="shared" si="80"/>
-        <v>19001</v>
-      </c>
-    </row>
-    <row r="1334" spans="8:17" ht="15.75" customHeight="1">
-      <c r="H1334">
-        <f t="shared" si="85"/>
-        <v>0</v>
-      </c>
-      <c r="I1334">
-        <f t="shared" si="81"/>
-        <v>0</v>
-      </c>
-      <c r="J1334">
-        <f t="shared" si="82"/>
-        <v>0</v>
-      </c>
-      <c r="K1334">
-        <f t="shared" si="83"/>
-        <v>0</v>
-      </c>
-      <c r="P1334" t="b">
-        <f t="shared" si="84"/>
-        <v>1</v>
-      </c>
-      <c r="Q1334" t="str">
-        <f t="shared" si="80"/>
-        <v>19001</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:Q1334">
+  <autoFilter ref="A1:Q1332">
     <filterColumn colId="1"/>
     <filterColumn colId="2"/>
   </autoFilter>

</xml_diff>